<commit_message>
change to S File 1
</commit_message>
<xml_diff>
--- a/SupplementaryFile1.xlsx
+++ b/SupplementaryFile1.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576706D-DFF2-4223-A207-9EE32895F380}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9827B1D2-676C-4D37-8DD4-8D79C464EED3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="JCV matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="clusters" sheetId="2" r:id="rId2"/>
-    <sheet name="stats" sheetId="3" r:id="rId3"/>
+    <sheet name="species" sheetId="4" r:id="rId1"/>
+    <sheet name="JCV matrix" sheetId="1" r:id="rId2"/>
+    <sheet name="clusters" sheetId="2" r:id="rId3"/>
+    <sheet name="stats" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Chlamydomonas_eustigmata</t>
   </si>
@@ -79,6 +80,51 @@
   </si>
   <si>
     <t>6.8x10-13</t>
+  </si>
+  <si>
+    <t>Uniprot ID</t>
+  </si>
+  <si>
+    <t>no. proteins</t>
+  </si>
+  <si>
+    <t>no. mapped</t>
+  </si>
+  <si>
+    <t>Chlamydomonas reinhardtii</t>
+  </si>
+  <si>
+    <t>Chlamydomonas eustigmata</t>
+  </si>
+  <si>
+    <t>Micromonas pusilla</t>
+  </si>
+  <si>
+    <t>Micromonas commoda</t>
+  </si>
+  <si>
+    <t>Saccharomyces cerevisiae</t>
+  </si>
+  <si>
+    <t>Volvox carteri f. nagariensis</t>
+  </si>
+  <si>
+    <t>UP000001058</t>
+  </si>
+  <si>
+    <t>UP000006906</t>
+  </si>
+  <si>
+    <t>UP000232323</t>
+  </si>
+  <si>
+    <t>UP000001876</t>
+  </si>
+  <si>
+    <t>UP000002009</t>
+  </si>
+  <si>
+    <t>UP000002311</t>
   </si>
 </sst>
 </file>
@@ -407,6 +453,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7630BDFA-D38D-49E4-BC89-4C24896544DE}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>14139</v>
+      </c>
+      <c r="D2">
+        <v>6243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>18828</v>
+      </c>
+      <c r="D3">
+        <v>7926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>10115</v>
+      </c>
+      <c r="D4">
+        <v>6893</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>10250</v>
+      </c>
+      <c r="D5">
+        <v>5786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>6049</v>
+      </c>
+      <c r="D6">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>14335</v>
+      </c>
+      <c r="D7">
+        <v>8181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -581,7 +745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2941F7E6-4E5F-4D6A-94AC-9ED230B59D88}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -653,11 +817,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B67F85-9661-4398-80EB-FE6B1FFE59D0}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
added 3 more species
</commit_message>
<xml_diff>
--- a/SupplementaryFile1.xlsx
+++ b/SupplementaryFile1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9827B1D2-676C-4D37-8DD4-8D79C464EED3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FFF7C0-2D89-4172-86B4-3009C4871FB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,6 +14,7 @@
     <sheet name="stats" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Chlamydomonas_eustigmata</t>
   </si>
@@ -79,9 +80,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>6.8x10-13</t>
-  </si>
-  <si>
     <t>Uniprot ID</t>
   </si>
   <si>
@@ -125,6 +123,27 @@
   </si>
   <si>
     <t>UP000002311</t>
+  </si>
+  <si>
+    <t>Gonium pectorale</t>
+  </si>
+  <si>
+    <t>UP000075714</t>
+  </si>
+  <si>
+    <t>Chlorella_sorokiniana</t>
+  </si>
+  <si>
+    <t>Chlorella_variabilis</t>
+  </si>
+  <si>
+    <t>UP000239899</t>
+  </si>
+  <si>
+    <t>UP000008141</t>
+  </si>
+  <si>
+    <t>Gonium_pectorale</t>
   </si>
 </sst>
 </file>
@@ -168,10 +187,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -454,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7630BDFA-D38D-49E4-BC89-4C24896544DE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,96 +494,138 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2">
-        <v>14139</v>
+        <v>10201</v>
       </c>
       <c r="D2">
-        <v>6243</v>
+        <v>4746</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C3">
-        <v>18828</v>
+        <v>9831</v>
       </c>
       <c r="D3">
-        <v>7926</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4">
-        <v>10115</v>
+        <v>14139</v>
       </c>
       <c r="D4">
-        <v>6893</v>
+        <v>6243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>10250</v>
+        <v>18828</v>
       </c>
       <c r="D5">
-        <v>5786</v>
+        <v>7926</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>6049</v>
+        <v>16224</v>
       </c>
       <c r="D6">
-        <v>4537</v>
+        <v>6815</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>10115</v>
+      </c>
+      <c r="D7">
+        <v>6893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>10250</v>
+      </c>
+      <c r="D8">
+        <v>5786</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>6049</v>
+      </c>
+      <c r="D9">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7">
+      <c r="C10">
         <v>14335</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>8181</v>
       </c>
     </row>
@@ -572,16 +637,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,19 +655,28 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,19 +687,28 @@
         <v>0.60956492104964199</v>
       </c>
       <c r="D2">
+        <v>0.52688620258440999</v>
+      </c>
+      <c r="E2">
+        <v>0.52608108108108098</v>
+      </c>
+      <c r="F2">
+        <v>0.61668936486319204</v>
+      </c>
+      <c r="G2">
         <v>0.45101071468021697</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>0.46124878522837698</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>0.22891016871865</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>0.57192676547515298</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,107 +719,248 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="E3">
+        <v>0.46803937096956699</v>
+      </c>
+      <c r="F3">
+        <v>0.72207943925233598</v>
+      </c>
+      <c r="G3">
         <v>0.39881064753634099</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>0.395623409669211</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>0.195721001631008</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>0.69797596457938005</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>0.52688620258440999</v>
+      </c>
+      <c r="C4">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.69657083477658499</v>
+      </c>
+      <c r="F4">
+        <v>0.47011698880976599</v>
+      </c>
+      <c r="G4">
+        <v>0.4207763671875</v>
+      </c>
+      <c r="H4">
+        <v>0.45409360762115097</v>
+      </c>
+      <c r="I4">
+        <v>0.25310475161987001</v>
+      </c>
+      <c r="J4">
+        <v>0.41309575863576697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>0.52608108108108098</v>
+      </c>
+      <c r="C5">
+        <v>0.46803937096956699</v>
+      </c>
+      <c r="D5">
+        <v>0.69657083477658499</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.471901749162635</v>
+      </c>
+      <c r="G5">
+        <v>0.42705221651332298</v>
+      </c>
+      <c r="H5">
+        <v>0.45274165437726199</v>
+      </c>
+      <c r="I5">
+        <v>0.24684614384185199</v>
+      </c>
+      <c r="J5">
+        <v>0.41978753085095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>0.61668936486319204</v>
+      </c>
+      <c r="C6">
+        <v>0.72207943925233598</v>
+      </c>
+      <c r="D6">
+        <v>0.47011698880976599</v>
+      </c>
+      <c r="E6">
+        <v>0.471901749162635</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.39139261063743402</v>
+      </c>
+      <c r="H6">
+        <v>0.396077996897851</v>
+      </c>
+      <c r="I6">
+        <v>0.20139697322468</v>
+      </c>
+      <c r="J6">
+        <v>0.67235418757666998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>0.45101071468021697</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>0.39881064753634099</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="D7">
+        <v>0.4207763671875</v>
+      </c>
+      <c r="E7">
+        <v>0.42705221651332298</v>
+      </c>
+      <c r="F7">
+        <v>0.39139261063743402</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.75003450655624604</v>
       </c>
-      <c r="F4">
+      <c r="I7">
         <v>0.21556949909603301</v>
       </c>
-      <c r="G4">
+      <c r="J7">
         <v>0.36887032328369102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>0.46124878522837698</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>0.395623409669211</v>
       </c>
-      <c r="D5">
+      <c r="D8">
+        <v>0.45409360762115097</v>
+      </c>
+      <c r="E8">
+        <v>0.45274165437726199</v>
+      </c>
+      <c r="F8">
+        <v>0.396077996897851</v>
+      </c>
+      <c r="G8">
         <v>0.75003450655624604</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0.22557283628161001</v>
       </c>
-      <c r="G5">
+      <c r="J8">
         <v>0.36503127443315098</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>0.22891016871865</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>0.195721001631008</v>
       </c>
-      <c r="D6">
+      <c r="D9">
+        <v>0.25310475161987001</v>
+      </c>
+      <c r="E9">
+        <v>0.24684614384185199</v>
+      </c>
+      <c r="F9">
+        <v>0.20139697322468</v>
+      </c>
+      <c r="G9">
         <v>0.21556949909603301</v>
       </c>
-      <c r="E6">
+      <c r="H9">
         <v>0.22557283628161001</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>0.187821051648454</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>0.57192676547515298</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>0.69797596457938005</v>
       </c>
-      <c r="D7">
+      <c r="D10">
+        <v>0.41309575863576697</v>
+      </c>
+      <c r="E10">
+        <v>0.41978753085095</v>
+      </c>
+      <c r="F10">
+        <v>0.67235418757666998</v>
+      </c>
+      <c r="G10">
         <v>0.36887032328369102</v>
       </c>
-      <c r="E7">
+      <c r="H10">
         <v>0.36503127443315098</v>
       </c>
-      <c r="F7">
+      <c r="I10">
         <v>0.187821051648454</v>
       </c>
-      <c r="G7">
+      <c r="J10">
         <v>1</v>
       </c>
     </row>
@@ -747,7 +972,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2941F7E6-4E5F-4D6A-94AC-9ED230B59D88}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,49 +991,73 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
     </row>
@@ -819,7 +1068,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B67F85-9661-4398-80EB-FE6B1FFE59D0}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -853,22 +1102,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>0.626</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="D2">
-        <v>6.5000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E2">
         <v>0.57199999999999995</v>
       </c>
       <c r="F2">
-        <v>0.69799999999999995</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="G2">
-        <v>2.68879898246417E-2</v>
+        <v>1.24298501407396E-4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -890,8 +1139,31 @@
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
+      <c r="G3" s="4">
+        <v>2.276E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.69657083477658499</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.0759999999999999E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>